<commit_message>
dodanie daty kiedy nie ma przyspieszenia z danej predkosci
</commit_message>
<xml_diff>
--- a/Raw files GPS/Raw files GPS Zagłębie/poniedziałek/wyniki/wyniki_Adamczyk_27.01.2025_9.xlsx
+++ b/Raw files GPS/Raw files GPS Zagłębie/poniedziałek/wyniki/wyniki_Adamczyk_27.01.2025_9.xlsx
@@ -461,7 +461,11 @@
       </c>
     </row>
     <row r="2">
-      <c r="A2" t="inlineStr"/>
+      <c r="A2" t="inlineStr">
+        <is>
+          <t>27.01.2025</t>
+        </is>
+      </c>
       <c r="B2" t="inlineStr"/>
       <c r="C2" t="inlineStr"/>
       <c r="D2" t="inlineStr"/>
@@ -472,7 +476,11 @@
       </c>
     </row>
     <row r="3">
-      <c r="A3" t="inlineStr"/>
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>27.01.2025</t>
+        </is>
+      </c>
       <c r="B3" t="inlineStr"/>
       <c r="C3" t="inlineStr"/>
       <c r="D3" t="inlineStr"/>

</xml_diff>